<commit_message>
Added main.py and added send mesage, compare time, and get weekday functionality to schedule.Schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethankisiel/Desktop/Schedule Notifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3ACBAC0-85F8-4C49-BE7C-8172CAA65B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D771230E-45F5-E84E-B504-31C3C6FDEE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26680" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -591,7 +591,7 @@
   <dimension ref="B1:J52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Added functionality to main.py
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethankisiel/Desktop/Schedule Notifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D771230E-45F5-E84E-B504-31C3C6FDEE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C019A19C-CC2A-9747-9AB2-2F2BA16C4CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26680" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="21">
   <si>
     <t>Daily Schedule</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Lunch</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -590,8 +593,8 @@
   </sheetPr>
   <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1097,7 +1100,7 @@
     </row>
     <row r="32" spans="2:9" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="11">
-        <f t="shared" si="0"/>
+        <f>B31+TIME(0,30,0)</f>
         <v>0.77083333333333359</v>
       </c>
       <c r="C32" s="12"/>
@@ -1110,7 +1113,7 @@
     </row>
     <row r="33" spans="2:9" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="11">
-        <f t="shared" si="0"/>
+        <f>B32+TIME(0,30,0)</f>
         <v>0.79166666666666696</v>
       </c>
       <c r="C33" s="12"/>
@@ -1123,7 +1126,7 @@
     </row>
     <row r="34" spans="2:9" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="11">
-        <f t="shared" si="0"/>
+        <f>B33+TIME(0,30,0)</f>
         <v>0.81250000000000033</v>
       </c>
       <c r="C34" s="12"/>
@@ -1139,7 +1142,9 @@
         <f t="shared" si="0"/>
         <v>0.8333333333333337</v>
       </c>
-      <c r="C35" s="12"/>
+      <c r="C35" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>

</xml_diff>

<commit_message>
updated to use Twilio instead of email sms gate for more reliable message delivery
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethankisiel/Desktop/Schedule Notifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C019A19C-CC2A-9747-9AB2-2F2BA16C4CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CA49DD-00AB-8A44-A0AA-43C251B126C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26680" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
   <si>
     <t>Daily Schedule</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Read News</t>
   </si>
   <si>
-    <t>Begin Studies</t>
-  </si>
-  <si>
     <t>Read SCIP</t>
   </si>
   <si>
@@ -99,7 +96,16 @@
     <t>Lunch</t>
   </si>
   <si>
-    <t>TEST</t>
+    <t>Single Var Calc</t>
+  </si>
+  <si>
+    <t>EdX</t>
+  </si>
+  <si>
+    <t>BED</t>
+  </si>
+  <si>
+    <t>Leisure Reading</t>
   </si>
 </sst>
 </file>
@@ -197,7 +203,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -243,6 +249,9 @@
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -593,8 +602,8 @@
   </sheetPr>
   <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -788,25 +797,25 @@
         <v>0.35416666666666657</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -841,25 +850,25 @@
         <v>0.41666666666666652</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -867,27 +876,13 @@
         <f t="shared" si="0"/>
         <v>0.43749999999999983</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>17</v>
-      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" spans="2:9" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="11">
@@ -921,25 +916,25 @@
         <v>0.49999999999999978</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -947,13 +942,27 @@
         <f t="shared" si="0"/>
         <v>0.52083333333333315</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="21" spans="2:9" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="11">
@@ -1038,13 +1047,27 @@
         <f t="shared" si="0"/>
         <v>0.66666666666666674</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
+      <c r="C27" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="28" spans="2:9" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="11">
@@ -1142,9 +1165,7 @@
         <f t="shared" si="0"/>
         <v>0.8333333333333337</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -1183,13 +1204,27 @@
         <f t="shared" si="0"/>
         <v>0.89583333333333381</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
+      <c r="C38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="39" spans="2:9" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="11">
@@ -1209,13 +1244,27 @@
         <f t="shared" si="1"/>
         <v>0.93750000000000056</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
+      <c r="C40" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="41" spans="2:9" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="11">

</xml_diff>